<commit_message>
Updating DAC baseline costs
</commit_message>
<xml_diff>
--- a/SubRes_Tmpl/SubRES_CCUS.xlsx
+++ b/SubRes_Tmpl/SubRES_CCUS.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SubRes_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F49696-5543-471E-B83B-BFA905A4466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0140F74-AD1B-4AB4-BED0-1ACAA4621599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="3384" windowWidth="25476" windowHeight="11688" xr2:uid="{D7A8135B-8EF1-4730-8204-54F3CFCE917E}"/>
+    <workbookView xWindow="2620" yWindow="2620" windowWidth="14400" windowHeight="8170" xr2:uid="{D7A8135B-8EF1-4730-8204-54F3CFCE917E}"/>
   </bookViews>
   <sheets>
     <sheet name="SUP_DAC" sheetId="1" r:id="rId1"/>
+    <sheet name="Sources" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -432,7 +433,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
   <si>
     <t>TechName</t>
   </si>
@@ -627,6 +628,9 @@
   </si>
   <si>
     <t>kt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sources </t>
   </si>
 </sst>
 </file>
@@ -1084,39 +1088,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E689EB1-03C8-41DF-9F76-ED40607CBFAA}">
   <dimension ref="B4:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8"/>
+    <sheetView tabSelected="1" topLeftCell="R7" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.08984375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="5" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:28" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:28" ht="29" x14ac:dyDescent="0.35">
       <c r="E4" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1203,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:28" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:28" ht="26" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1272,7 +1276,7 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>32</v>
       </c>
@@ -1348,13 +1352,13 @@
         <v>25</v>
       </c>
       <c r="AA7">
-        <v>2025</v>
+        <v>2100</v>
       </c>
       <c r="AB7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:28" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>37</v>
       </c>
@@ -1374,7 +1378,7 @@
         <v>1.0329440232461128E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:28" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>38</v>
       </c>
@@ -1394,7 +1398,7 @@
         <v>4.7515425069321188E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:28" x14ac:dyDescent="0.35">
       <c r="E10" t="s">
         <v>40</v>
       </c>
@@ -1402,7 +1406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:28" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -1478,13 +1482,13 @@
         <v>25</v>
       </c>
       <c r="AA11">
-        <v>2100</v>
+        <v>2025</v>
       </c>
       <c r="AB11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:28" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>37</v>
       </c>
@@ -1504,7 +1508,7 @@
         <v>1.0329440232461128E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:28" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>36</v>
       </c>
@@ -1524,7 +1528,7 @@
         <v>4.7515425069321188E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:28" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>40</v>
       </c>
@@ -1532,10 +1536,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="L20" s="8"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="7" t="s">
         <v>55</v>
       </c>
@@ -1547,7 +1551,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="4" t="s">
         <v>56</v>
       </c>
@@ -1573,7 +1577,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" ht="39" x14ac:dyDescent="0.35">
       <c r="B24" s="5" t="s">
         <v>57</v>
       </c>
@@ -1599,7 +1603,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
         <v>59</v>
       </c>
@@ -1618,12 +1622,10 @@
       <c r="G25" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="H25" s="6"/>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
         <v>59</v>
       </c>
@@ -1642,10 +1644,7 @@
       <c r="G26" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="6" t="str">
-        <f>H25</f>
-        <v>CO2Captured</v>
-      </c>
+      <c r="H26" s="6"/>
       <c r="I26" s="6"/>
     </row>
   </sheetData>
@@ -1653,4 +1652,24 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB0C080-7CBD-4C6D-A6A6-22303027DB5C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>